<commit_message>
excel-sheet reeds gereed bijgewerkt
</commit_message>
<xml_diff>
--- a/1.0.4-matrix-1.3-rc/matrix/Validatiematrix_v1.3-rc.xlsx
+++ b/1.0.4-matrix-1.3-rc/matrix/Validatiematrix_v1.3-rc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4-matrix-1.3-rc\matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C280F5-F55E-44E7-A5D0-3AEF556D0E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01E9C24-97E3-4A3B-BBBD-6370AB5BC35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Validatieregels" sheetId="14" r:id="rId1"/>
@@ -6328,7 +6328,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6355,13 +6355,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6819,25 +6825,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -9751,10 +9757,10 @@
   <dimension ref="A1:O734"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D592" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C158" sqref="C158"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9920,7 +9926,7 @@
       <c r="B4" s="38">
         <v>2</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="81" t="s">
         <v>1012</v>
       </c>
       <c r="D4" s="18" t="s">
@@ -9968,7 +9974,7 @@
       <c r="B5" s="38">
         <v>2</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="81" t="s">
         <v>1013</v>
       </c>
       <c r="D5" s="18" t="s">
@@ -10016,7 +10022,7 @@
       <c r="B6" s="38">
         <v>2</v>
       </c>
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="81" t="s">
         <v>1014</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -10064,7 +10070,7 @@
       <c r="B7" s="38">
         <v>2</v>
       </c>
-      <c r="C7" s="77" t="s">
+      <c r="C7" s="81" t="s">
         <v>1015</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -10112,7 +10118,7 @@
       <c r="B8" s="38">
         <v>2</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="81" t="s">
         <v>1016</v>
       </c>
       <c r="D8" s="18" t="s">
@@ -10160,7 +10166,7 @@
       <c r="B9" s="38">
         <v>2</v>
       </c>
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="81" t="s">
         <v>1017</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -10208,7 +10214,7 @@
       <c r="B10" s="38">
         <v>2</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="81" t="s">
         <v>1018</v>
       </c>
       <c r="D10" s="18" t="s">
@@ -10256,7 +10262,7 @@
       <c r="B11" s="38">
         <v>2</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="81" t="s">
         <v>1019</v>
       </c>
       <c r="D11" s="18" t="s">
@@ -10304,7 +10310,7 @@
       <c r="B12" s="38">
         <v>2</v>
       </c>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="81" t="s">
         <v>1020</v>
       </c>
       <c r="D12" s="18" t="s">
@@ -10352,7 +10358,7 @@
       <c r="B13" s="38">
         <v>2</v>
       </c>
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="81" t="s">
         <v>1021</v>
       </c>
       <c r="D13" s="18" t="s">
@@ -10400,7 +10406,7 @@
       <c r="B14" s="38">
         <v>2</v>
       </c>
-      <c r="C14" s="77" t="s">
+      <c r="C14" s="81" t="s">
         <v>1022</v>
       </c>
       <c r="D14" s="18" t="s">
@@ -10448,7 +10454,7 @@
       <c r="B15" s="38">
         <v>2</v>
       </c>
-      <c r="C15" s="77" t="s">
+      <c r="C15" s="81" t="s">
         <v>1023</v>
       </c>
       <c r="D15" s="18" t="s">
@@ -10496,7 +10502,7 @@
       <c r="B16" s="38">
         <v>2</v>
       </c>
-      <c r="C16" s="77" t="s">
+      <c r="C16" s="81" t="s">
         <v>1024</v>
       </c>
       <c r="D16" s="18" t="s">
@@ -10544,7 +10550,7 @@
       <c r="B17" s="38">
         <v>2</v>
       </c>
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="81" t="s">
         <v>1025</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -10592,7 +10598,7 @@
       <c r="B18" s="38">
         <v>2</v>
       </c>
-      <c r="C18" s="77" t="s">
+      <c r="C18" s="81" t="s">
         <v>1026</v>
       </c>
       <c r="D18" s="18" t="s">
@@ -10928,7 +10934,7 @@
       <c r="B25" s="38">
         <v>2</v>
       </c>
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="81" t="s">
         <v>1890</v>
       </c>
       <c r="D25" s="18" t="s">
@@ -10975,7 +10981,7 @@
       <c r="B26" s="38">
         <v>2</v>
       </c>
-      <c r="C26" s="77" t="s">
+      <c r="C26" s="81" t="s">
         <v>1891</v>
       </c>
       <c r="D26" s="18" t="s">
@@ -11022,7 +11028,7 @@
       <c r="B27" s="38">
         <v>4</v>
       </c>
-      <c r="C27" s="77" t="s">
+      <c r="C27" s="81" t="s">
         <v>1388</v>
       </c>
       <c r="D27" s="18" t="s">
@@ -11070,7 +11076,7 @@
       <c r="B28" s="38">
         <v>4</v>
       </c>
-      <c r="C28" s="77" t="s">
+      <c r="C28" s="81" t="s">
         <v>1390</v>
       </c>
       <c r="D28" s="18" t="s">
@@ -11118,7 +11124,7 @@
       <c r="B29" s="38">
         <v>4</v>
       </c>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="81" t="s">
         <v>1392</v>
       </c>
       <c r="D29" s="18" t="s">
@@ -11166,7 +11172,7 @@
       <c r="B30" s="38">
         <v>4</v>
       </c>
-      <c r="C30" s="77" t="s">
+      <c r="C30" s="81" t="s">
         <v>1394</v>
       </c>
       <c r="D30" s="18" t="s">
@@ -11214,7 +11220,7 @@
       <c r="B31" s="38">
         <v>4</v>
       </c>
-      <c r="C31" s="77" t="s">
+      <c r="C31" s="81" t="s">
         <v>1396</v>
       </c>
       <c r="D31" s="18" t="s">
@@ -11262,7 +11268,7 @@
       <c r="B32" s="38">
         <v>4</v>
       </c>
-      <c r="C32" s="77" t="s">
+      <c r="C32" s="81" t="s">
         <v>1398</v>
       </c>
       <c r="D32" s="18" t="s">
@@ -11310,7 +11316,7 @@
       <c r="B33" s="44">
         <v>4</v>
       </c>
-      <c r="C33" s="77" t="s">
+      <c r="C33" s="81" t="s">
         <v>1400</v>
       </c>
       <c r="D33" s="18" t="s">
@@ -11358,7 +11364,7 @@
       <c r="B34" s="44">
         <v>4</v>
       </c>
-      <c r="C34" s="77" t="s">
+      <c r="C34" s="81" t="s">
         <v>1402</v>
       </c>
       <c r="D34" s="18" t="s">
@@ -11406,7 +11412,7 @@
       <c r="B35" s="44">
         <v>4</v>
       </c>
-      <c r="C35" s="77" t="s">
+      <c r="C35" s="81" t="s">
         <v>1404</v>
       </c>
       <c r="D35" s="18" t="s">
@@ -11454,7 +11460,7 @@
       <c r="B36" s="44">
         <v>4</v>
       </c>
-      <c r="C36" s="77" t="s">
+      <c r="C36" s="81" t="s">
         <v>1406</v>
       </c>
       <c r="D36" s="18" t="s">
@@ -11502,7 +11508,7 @@
       <c r="B37" s="44">
         <v>4</v>
       </c>
-      <c r="C37" s="77" t="s">
+      <c r="C37" s="81" t="s">
         <v>1408</v>
       </c>
       <c r="D37" s="18" t="s">
@@ -11550,7 +11556,7 @@
       <c r="B38" s="44">
         <v>4</v>
       </c>
-      <c r="C38" s="77" t="s">
+      <c r="C38" s="81" t="s">
         <v>1410</v>
       </c>
       <c r="D38" s="18" t="s">
@@ -11598,7 +11604,7 @@
       <c r="B39" s="38">
         <v>4</v>
       </c>
-      <c r="C39" s="77" t="s">
+      <c r="C39" s="81" t="s">
         <v>673</v>
       </c>
       <c r="D39" s="18" t="s">
@@ -11646,7 +11652,7 @@
       <c r="B40" s="38">
         <v>4</v>
       </c>
-      <c r="C40" s="77" t="s">
+      <c r="C40" s="81" t="s">
         <v>1255</v>
       </c>
       <c r="D40" s="18" t="s">
@@ -11694,7 +11700,7 @@
       <c r="B41" s="38">
         <v>4</v>
       </c>
-      <c r="C41" s="77" t="s">
+      <c r="C41" s="81" t="s">
         <v>674</v>
       </c>
       <c r="D41" s="18" t="s">
@@ -11742,7 +11748,7 @@
       <c r="B42" s="38">
         <v>4</v>
       </c>
-      <c r="C42" s="77" t="s">
+      <c r="C42" s="81" t="s">
         <v>675</v>
       </c>
       <c r="D42" s="18" t="s">
@@ -11934,7 +11940,7 @@
       <c r="B46" s="38">
         <v>1</v>
       </c>
-      <c r="C46" s="78" t="s">
+      <c r="C46" s="82" t="s">
         <v>27</v>
       </c>
       <c r="D46" s="18" t="s">
@@ -11982,7 +11988,7 @@
       <c r="B47" s="38">
         <v>1</v>
       </c>
-      <c r="C47" s="78" t="s">
+      <c r="C47" s="82" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="18" t="s">
@@ -12030,7 +12036,7 @@
       <c r="B48" s="38">
         <v>1</v>
       </c>
-      <c r="C48" s="78" t="s">
+      <c r="C48" s="82" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="18" t="s">
@@ -12078,7 +12084,7 @@
       <c r="B49" s="38">
         <v>1</v>
       </c>
-      <c r="C49" s="78" t="s">
+      <c r="C49" s="82" t="s">
         <v>30</v>
       </c>
       <c r="D49" s="18" t="s">
@@ -12174,7 +12180,7 @@
       <c r="B51" s="38">
         <v>1</v>
       </c>
-      <c r="C51" s="78" t="s">
+      <c r="C51" s="82" t="s">
         <v>32</v>
       </c>
       <c r="D51" s="18" t="s">
@@ -12270,7 +12276,7 @@
       <c r="B53" s="38">
         <v>1</v>
       </c>
-      <c r="C53" s="78" t="s">
+      <c r="C53" s="82" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="18" t="s">
@@ -12318,7 +12324,7 @@
       <c r="B54" s="38">
         <v>1</v>
       </c>
-      <c r="C54" s="78" t="s">
+      <c r="C54" s="82" t="s">
         <v>35</v>
       </c>
       <c r="D54" s="18" t="s">
@@ -12366,7 +12372,7 @@
       <c r="B55" s="38">
         <v>1</v>
       </c>
-      <c r="C55" s="78" t="s">
+      <c r="C55" s="82" t="s">
         <v>36</v>
       </c>
       <c r="D55" s="18" t="s">
@@ -12459,7 +12465,7 @@
       <c r="A57" s="38" t="s">
         <v>1820</v>
       </c>
-      <c r="B57" s="79">
+      <c r="B57" s="77">
         <v>1</v>
       </c>
       <c r="C57" s="22" t="s">
@@ -12509,7 +12515,7 @@
       <c r="B58" s="38">
         <v>1</v>
       </c>
-      <c r="C58" s="78" t="s">
+      <c r="C58" s="82" t="s">
         <v>39</v>
       </c>
       <c r="D58" s="18" t="s">
@@ -12557,7 +12563,7 @@
       <c r="B59" s="38">
         <v>1</v>
       </c>
-      <c r="C59" s="78" t="s">
+      <c r="C59" s="82" t="s">
         <v>68</v>
       </c>
       <c r="D59" s="18" t="s">
@@ -12605,7 +12611,7 @@
       <c r="B60" s="38">
         <v>1</v>
       </c>
-      <c r="C60" s="78" t="s">
+      <c r="C60" s="82" t="s">
         <v>70</v>
       </c>
       <c r="D60" s="18" t="s">
@@ -12653,7 +12659,7 @@
       <c r="B61" s="38">
         <v>1</v>
       </c>
-      <c r="C61" s="78" t="s">
+      <c r="C61" s="82" t="s">
         <v>72</v>
       </c>
       <c r="D61" s="18" t="s">
@@ -12701,7 +12707,7 @@
       <c r="B62" s="38">
         <v>1</v>
       </c>
-      <c r="C62" s="78" t="s">
+      <c r="C62" s="82" t="s">
         <v>74</v>
       </c>
       <c r="D62" s="18" t="s">
@@ -12749,7 +12755,7 @@
       <c r="B63" s="38">
         <v>1</v>
       </c>
-      <c r="C63" s="78" t="s">
+      <c r="C63" s="82" t="s">
         <v>76</v>
       </c>
       <c r="D63" s="18" t="s">
@@ -12797,7 +12803,7 @@
       <c r="B64" s="38">
         <v>1</v>
       </c>
-      <c r="C64" s="78" t="s">
+      <c r="C64" s="82" t="s">
         <v>77</v>
       </c>
       <c r="D64" s="18" t="s">
@@ -12845,7 +12851,7 @@
       <c r="B65" s="38">
         <v>1</v>
       </c>
-      <c r="C65" s="78" t="s">
+      <c r="C65" s="82" t="s">
         <v>79</v>
       </c>
       <c r="D65" s="18" t="s">
@@ -13133,7 +13139,7 @@
       <c r="B71" s="73">
         <v>2</v>
       </c>
-      <c r="C71" s="77" t="s">
+      <c r="C71" s="81" t="s">
         <v>1269</v>
       </c>
       <c r="D71" s="18" t="s">
@@ -13187,7 +13193,7 @@
       <c r="B72" s="73">
         <v>2</v>
       </c>
-      <c r="C72" s="77" t="s">
+      <c r="C72" s="81" t="s">
         <v>1824</v>
       </c>
       <c r="D72" s="18" t="s">
@@ -13241,7 +13247,7 @@
       <c r="B73" s="38">
         <v>2</v>
       </c>
-      <c r="C73" s="78" t="s">
+      <c r="C73" s="82" t="s">
         <v>147</v>
       </c>
       <c r="D73" s="18" t="s">
@@ -13388,7 +13394,7 @@
       <c r="B76" s="38">
         <v>2</v>
       </c>
-      <c r="C76" s="77" t="s">
+      <c r="C76" s="81" t="s">
         <v>1067</v>
       </c>
       <c r="D76" s="18" t="s">
@@ -13435,7 +13441,7 @@
       <c r="B77" s="38">
         <v>2</v>
       </c>
-      <c r="C77" s="78" t="s">
+      <c r="C77" s="82" t="s">
         <v>149</v>
       </c>
       <c r="D77" s="18" t="s">
@@ -13629,7 +13635,7 @@
       <c r="B81" s="38">
         <v>2</v>
       </c>
-      <c r="C81" s="78" t="s">
+      <c r="C81" s="82" t="s">
         <v>694</v>
       </c>
       <c r="D81" s="18" t="s">
@@ -13676,7 +13682,7 @@
       <c r="B82" s="38">
         <v>2</v>
       </c>
-      <c r="C82" s="78" t="s">
+      <c r="C82" s="82" t="s">
         <v>696</v>
       </c>
       <c r="D82" s="18" t="s">
@@ -17307,7 +17313,7 @@
       <c r="B158" s="74">
         <v>2</v>
       </c>
-      <c r="C158" s="18" t="s">
+      <c r="C158" s="81" t="s">
         <v>1091</v>
       </c>
       <c r="D158" s="18" t="s">
@@ -17403,7 +17409,7 @@
       <c r="B160" s="72">
         <v>2</v>
       </c>
-      <c r="C160" s="38" t="s">
+      <c r="C160" s="82" t="s">
         <v>1286</v>
       </c>
       <c r="D160" s="22" t="s">
@@ -17451,7 +17457,7 @@
       <c r="B161" s="72">
         <v>2</v>
       </c>
-      <c r="C161" s="38" t="s">
+      <c r="C161" s="82" t="s">
         <v>1288</v>
       </c>
       <c r="D161" s="22" t="s">
@@ -17547,7 +17553,7 @@
       <c r="B163" s="38">
         <v>2</v>
       </c>
-      <c r="C163" s="22" t="s">
+      <c r="C163" s="82" t="s">
         <v>46</v>
       </c>
       <c r="D163" s="18" t="s">
@@ -17594,7 +17600,7 @@
       <c r="B164" s="74">
         <v>2</v>
       </c>
-      <c r="C164" s="18" t="s">
+      <c r="C164" s="81" t="s">
         <v>1095</v>
       </c>
       <c r="D164" s="18" t="s">
@@ -17642,7 +17648,7 @@
       <c r="B165" s="38">
         <v>2</v>
       </c>
-      <c r="C165" s="18" t="s">
+      <c r="C165" s="81" t="s">
         <v>1096</v>
       </c>
       <c r="D165" s="18" t="s">
@@ -17784,7 +17790,7 @@
       <c r="B168" s="38">
         <v>5</v>
       </c>
-      <c r="C168" s="22" t="s">
+      <c r="C168" s="82" t="s">
         <v>47</v>
       </c>
       <c r="D168" s="18" t="s">
@@ -18072,7 +18078,7 @@
       <c r="B174" s="38">
         <v>2</v>
       </c>
-      <c r="C174" s="22" t="s">
+      <c r="C174" s="82" t="s">
         <v>107</v>
       </c>
       <c r="D174" s="18" t="s">
@@ -18120,7 +18126,7 @@
       <c r="B175" s="38">
         <v>2</v>
       </c>
-      <c r="C175" s="22" t="s">
+      <c r="C175" s="82" t="s">
         <v>543</v>
       </c>
       <c r="D175" s="18" t="s">
@@ -18168,7 +18174,7 @@
       <c r="B176" s="38">
         <v>2</v>
       </c>
-      <c r="C176" s="22" t="s">
+      <c r="C176" s="82" t="s">
         <v>111</v>
       </c>
       <c r="D176" s="18" t="s">
@@ -18216,7 +18222,7 @@
       <c r="B177" s="38">
         <v>2</v>
       </c>
-      <c r="C177" s="22" t="s">
+      <c r="C177" s="82" t="s">
         <v>113</v>
       </c>
       <c r="D177" s="18" t="s">
@@ -18264,7 +18270,7 @@
       <c r="B178" s="38">
         <v>2</v>
       </c>
-      <c r="C178" s="22" t="s">
+      <c r="C178" s="82" t="s">
         <v>115</v>
       </c>
       <c r="D178" s="18" t="s">
@@ -18314,7 +18320,7 @@
       <c r="B179" s="38">
         <v>2</v>
       </c>
-      <c r="C179" s="22" t="s">
+      <c r="C179" s="82" t="s">
         <v>116</v>
       </c>
       <c r="D179" s="18" t="s">
@@ -18459,7 +18465,7 @@
       <c r="B182" s="38">
         <v>2</v>
       </c>
-      <c r="C182" s="22" t="s">
+      <c r="C182" s="82" t="s">
         <v>120</v>
       </c>
       <c r="D182" s="18" t="s">
@@ -18604,7 +18610,7 @@
       <c r="B185" s="38">
         <v>2</v>
       </c>
-      <c r="C185" s="22" t="s">
+      <c r="C185" s="82" t="s">
         <v>737</v>
       </c>
       <c r="D185" s="22" t="s">
@@ -18652,7 +18658,7 @@
       <c r="B186" s="38">
         <v>2</v>
       </c>
-      <c r="C186" s="22" t="s">
+      <c r="C186" s="82" t="s">
         <v>739</v>
       </c>
       <c r="D186" s="18" t="s">
@@ -19220,7 +19226,7 @@
       <c r="B197" s="38">
         <v>5</v>
       </c>
-      <c r="C197" s="38" t="s">
+      <c r="C197" s="82" t="s">
         <v>1310</v>
       </c>
       <c r="D197" s="22" t="s">
@@ -19363,7 +19369,7 @@
       <c r="B200" s="38">
         <v>5</v>
       </c>
-      <c r="C200" s="38" t="s">
+      <c r="C200" s="82" t="s">
         <v>1316</v>
       </c>
       <c r="D200" s="22" t="s">
@@ -19411,7 +19417,7 @@
       <c r="B201" s="38">
         <v>5</v>
       </c>
-      <c r="C201" s="38" t="s">
+      <c r="C201" s="82" t="s">
         <v>1319</v>
       </c>
       <c r="D201" s="22" t="s">
@@ -19555,7 +19561,7 @@
       <c r="B204" s="38">
         <v>5</v>
       </c>
-      <c r="C204" s="38" t="s">
+      <c r="C204" s="82" t="s">
         <v>1897</v>
       </c>
       <c r="D204" s="22" t="s">
@@ -19842,7 +19848,7 @@
       <c r="B210" s="38">
         <v>5</v>
       </c>
-      <c r="C210" s="38" t="s">
+      <c r="C210" s="82" t="s">
         <v>1343</v>
       </c>
       <c r="D210" s="22" t="s">
@@ -19889,7 +19895,7 @@
       <c r="B211" s="38">
         <v>5</v>
       </c>
-      <c r="C211" s="38" t="s">
+      <c r="C211" s="82" t="s">
         <v>1346</v>
       </c>
       <c r="D211" s="22" t="s">
@@ -20032,7 +20038,7 @@
       <c r="B214" s="38">
         <v>5</v>
       </c>
-      <c r="C214" s="38" t="s">
+      <c r="C214" s="82" t="s">
         <v>1355</v>
       </c>
       <c r="D214" s="22" t="s">
@@ -20176,7 +20182,7 @@
       <c r="B217" s="38">
         <v>5</v>
       </c>
-      <c r="C217" s="38" t="s">
+      <c r="C217" s="82" t="s">
         <v>1920</v>
       </c>
       <c r="D217" s="22" t="s">
@@ -20560,7 +20566,7 @@
       <c r="B225" s="38">
         <v>5</v>
       </c>
-      <c r="C225" s="22" t="s">
+      <c r="C225" s="82" t="s">
         <v>125</v>
       </c>
       <c r="D225" s="18" t="s">
@@ -20608,7 +20614,7 @@
       <c r="B226" s="38">
         <v>5</v>
       </c>
-      <c r="C226" s="22" t="s">
+      <c r="C226" s="82" t="s">
         <v>127</v>
       </c>
       <c r="D226" s="18" t="s">
@@ -20656,7 +20662,7 @@
       <c r="B227" s="38">
         <v>5</v>
       </c>
-      <c r="C227" s="22" t="s">
+      <c r="C227" s="82" t="s">
         <v>129</v>
       </c>
       <c r="D227" s="18" t="s">
@@ -21516,7 +21522,7 @@
       <c r="B245" s="38">
         <v>5</v>
       </c>
-      <c r="C245" s="18" t="s">
+      <c r="C245" s="81" t="s">
         <v>1058</v>
       </c>
       <c r="D245" s="18" t="s">
@@ -21563,7 +21569,7 @@
       <c r="B246" s="38">
         <v>5</v>
       </c>
-      <c r="C246" s="18" t="s">
+      <c r="C246" s="81" t="s">
         <v>1059</v>
       </c>
       <c r="D246" s="18" t="s">
@@ -21657,7 +21663,7 @@
       <c r="B248" s="38">
         <v>5</v>
       </c>
-      <c r="C248" s="18" t="s">
+      <c r="C248" s="80" t="s">
         <v>745</v>
       </c>
       <c r="D248" s="18" t="s">
@@ -21705,7 +21711,7 @@
       <c r="B249" s="38">
         <v>5</v>
       </c>
-      <c r="C249" s="18" t="s">
+      <c r="C249" s="80" t="s">
         <v>747</v>
       </c>
       <c r="D249" s="18" t="s">
@@ -21753,7 +21759,7 @@
       <c r="B250" s="38">
         <v>5</v>
       </c>
-      <c r="C250" s="18" t="s">
+      <c r="C250" s="81" t="s">
         <v>749</v>
       </c>
       <c r="D250" s="18" t="s">
@@ -21945,7 +21951,7 @@
       <c r="B254" s="38">
         <v>5</v>
       </c>
-      <c r="C254" s="18" t="s">
+      <c r="C254" s="81" t="s">
         <v>756</v>
       </c>
       <c r="D254" s="18" t="s">
@@ -22804,7 +22810,7 @@
       <c r="B272" s="38">
         <v>5</v>
       </c>
-      <c r="C272" s="18" t="s">
+      <c r="C272" s="81" t="s">
         <v>1152</v>
       </c>
       <c r="D272" s="18" t="s">
@@ -22852,7 +22858,7 @@
       <c r="B273" s="38">
         <v>5</v>
       </c>
-      <c r="C273" s="18" t="s">
+      <c r="C273" s="81" t="s">
         <v>1154</v>
       </c>
       <c r="D273" s="18" t="s">
@@ -23761,7 +23767,7 @@
       <c r="B292" s="38">
         <v>8</v>
       </c>
-      <c r="C292" s="18" t="s">
+      <c r="C292" s="81" t="s">
         <v>270</v>
       </c>
       <c r="D292" s="18" t="s">
@@ -23809,7 +23815,7 @@
       <c r="B293" s="38">
         <v>8</v>
       </c>
-      <c r="C293" s="18" t="s">
+      <c r="C293" s="81" t="s">
         <v>272</v>
       </c>
       <c r="D293" s="18" t="s">
@@ -23857,7 +23863,7 @@
       <c r="B294" s="38">
         <v>8</v>
       </c>
-      <c r="C294" s="18" t="s">
+      <c r="C294" s="81" t="s">
         <v>273</v>
       </c>
       <c r="D294" s="18" t="s">
@@ -23905,7 +23911,7 @@
       <c r="B295" s="38">
         <v>8</v>
       </c>
-      <c r="C295" s="18" t="s">
+      <c r="C295" s="81" t="s">
         <v>275</v>
       </c>
       <c r="D295" s="18" t="s">
@@ -23953,7 +23959,7 @@
       <c r="B296" s="38">
         <v>8</v>
       </c>
-      <c r="C296" s="18" t="s">
+      <c r="C296" s="81" t="s">
         <v>277</v>
       </c>
       <c r="D296" s="18" t="s">
@@ -24001,7 +24007,7 @@
       <c r="B297" s="38">
         <v>8</v>
       </c>
-      <c r="C297" s="18" t="s">
+      <c r="C297" s="81" t="s">
         <v>279</v>
       </c>
       <c r="D297" s="18" t="s">
@@ -24049,7 +24055,7 @@
       <c r="B298" s="38">
         <v>8</v>
       </c>
-      <c r="C298" s="18" t="s">
+      <c r="C298" s="81" t="s">
         <v>280</v>
       </c>
       <c r="D298" s="18" t="s">
@@ -24097,7 +24103,7 @@
       <c r="B299" s="38">
         <v>8</v>
       </c>
-      <c r="C299" s="18" t="s">
+      <c r="C299" s="81" t="s">
         <v>282</v>
       </c>
       <c r="D299" s="18" t="s">
@@ -24145,7 +24151,7 @@
       <c r="B300" s="38">
         <v>8</v>
       </c>
-      <c r="C300" s="18" t="s">
+      <c r="C300" s="81" t="s">
         <v>284</v>
       </c>
       <c r="D300" s="18" t="s">
@@ -24193,7 +24199,7 @@
       <c r="B301" s="38">
         <v>8</v>
       </c>
-      <c r="C301" s="18" t="s">
+      <c r="C301" s="81" t="s">
         <v>286</v>
       </c>
       <c r="D301" s="18" t="s">
@@ -24241,7 +24247,7 @@
       <c r="B302" s="38">
         <v>8</v>
       </c>
-      <c r="C302" s="18" t="s">
+      <c r="C302" s="81" t="s">
         <v>288</v>
       </c>
       <c r="D302" s="18" t="s">
@@ -24289,7 +24295,7 @@
       <c r="B303" s="38">
         <v>8</v>
       </c>
-      <c r="C303" s="18" t="s">
+      <c r="C303" s="81" t="s">
         <v>290</v>
       </c>
       <c r="D303" s="18" t="s">
@@ -24337,7 +24343,7 @@
       <c r="B304" s="38">
         <v>8</v>
       </c>
-      <c r="C304" s="18" t="s">
+      <c r="C304" s="81" t="s">
         <v>292</v>
       </c>
       <c r="D304" s="18" t="s">
@@ -24385,7 +24391,7 @@
       <c r="B305" s="38">
         <v>8</v>
       </c>
-      <c r="C305" s="18" t="s">
+      <c r="C305" s="81" t="s">
         <v>294</v>
       </c>
       <c r="D305" s="18" t="s">
@@ -24433,7 +24439,7 @@
       <c r="B306" s="38">
         <v>8</v>
       </c>
-      <c r="C306" s="18" t="s">
+      <c r="C306" s="81" t="s">
         <v>296</v>
       </c>
       <c r="D306" s="18" t="s">
@@ -24481,7 +24487,7 @@
       <c r="B307" s="38">
         <v>8</v>
       </c>
-      <c r="C307" s="18" t="s">
+      <c r="C307" s="81" t="s">
         <v>298</v>
       </c>
       <c r="D307" s="18" t="s">
@@ -24529,7 +24535,7 @@
       <c r="B308" s="38">
         <v>8</v>
       </c>
-      <c r="C308" s="18" t="s">
+      <c r="C308" s="81" t="s">
         <v>300</v>
       </c>
       <c r="D308" s="18" t="s">
@@ -24577,7 +24583,7 @@
       <c r="B309" s="38">
         <v>8</v>
       </c>
-      <c r="C309" s="18" t="s">
+      <c r="C309" s="81" t="s">
         <v>302</v>
       </c>
       <c r="D309" s="18" t="s">
@@ -24625,7 +24631,7 @@
       <c r="B310" s="38">
         <v>8</v>
       </c>
-      <c r="C310" s="18" t="s">
+      <c r="C310" s="81" t="s">
         <v>304</v>
       </c>
       <c r="D310" s="18" t="s">
@@ -24673,7 +24679,7 @@
       <c r="B311" s="38">
         <v>8</v>
       </c>
-      <c r="C311" s="18" t="s">
+      <c r="C311" s="81" t="s">
         <v>305</v>
       </c>
       <c r="D311" s="18" t="s">
@@ -24721,7 +24727,7 @@
       <c r="B312" s="38">
         <v>8</v>
       </c>
-      <c r="C312" s="18" t="s">
+      <c r="C312" s="81" t="s">
         <v>306</v>
       </c>
       <c r="D312" s="18" t="s">
@@ -24769,7 +24775,7 @@
       <c r="B313" s="38">
         <v>8</v>
       </c>
-      <c r="C313" s="18" t="s">
+      <c r="C313" s="81" t="s">
         <v>307</v>
       </c>
       <c r="D313" s="18" t="s">
@@ -24817,7 +24823,7 @@
       <c r="B314" s="38">
         <v>8</v>
       </c>
-      <c r="C314" s="18" t="s">
+      <c r="C314" s="81" t="s">
         <v>309</v>
       </c>
       <c r="D314" s="18" t="s">
@@ -24865,7 +24871,7 @@
       <c r="B315" s="38">
         <v>8</v>
       </c>
-      <c r="C315" s="18" t="s">
+      <c r="C315" s="81" t="s">
         <v>311</v>
       </c>
       <c r="D315" s="18" t="s">
@@ -24913,7 +24919,7 @@
       <c r="B316" s="38">
         <v>8</v>
       </c>
-      <c r="C316" s="18" t="s">
+      <c r="C316" s="81" t="s">
         <v>312</v>
       </c>
       <c r="D316" s="18" t="s">
@@ -24961,7 +24967,7 @@
       <c r="B317" s="38">
         <v>8</v>
       </c>
-      <c r="C317" s="18" t="s">
+      <c r="C317" s="81" t="s">
         <v>314</v>
       </c>
       <c r="D317" s="18" t="s">
@@ -25009,7 +25015,7 @@
       <c r="B318" s="38">
         <v>8</v>
       </c>
-      <c r="C318" s="18" t="s">
+      <c r="C318" s="81" t="s">
         <v>316</v>
       </c>
       <c r="D318" s="18" t="s">
@@ -25057,7 +25063,7 @@
       <c r="B319" s="38">
         <v>8</v>
       </c>
-      <c r="C319" s="18" t="s">
+      <c r="C319" s="81" t="s">
         <v>318</v>
       </c>
       <c r="D319" s="18" t="s">
@@ -25105,7 +25111,7 @@
       <c r="B320" s="38">
         <v>8</v>
       </c>
-      <c r="C320" s="18" t="s">
+      <c r="C320" s="81" t="s">
         <v>320</v>
       </c>
       <c r="D320" s="18" t="s">
@@ -25153,7 +25159,7 @@
       <c r="B321" s="38">
         <v>8</v>
       </c>
-      <c r="C321" s="18" t="s">
+      <c r="C321" s="81" t="s">
         <v>322</v>
       </c>
       <c r="D321" s="18" t="s">
@@ -25201,7 +25207,7 @@
       <c r="B322" s="38">
         <v>8</v>
       </c>
-      <c r="C322" s="18" t="s">
+      <c r="C322" s="81" t="s">
         <v>324</v>
       </c>
       <c r="D322" s="18" t="s">
@@ -25249,7 +25255,7 @@
       <c r="B323" s="38">
         <v>8</v>
       </c>
-      <c r="C323" s="18" t="s">
+      <c r="C323" s="81" t="s">
         <v>326</v>
       </c>
       <c r="D323" s="18" t="s">
@@ -25297,7 +25303,7 @@
       <c r="B324" s="38">
         <v>8</v>
       </c>
-      <c r="C324" s="18" t="s">
+      <c r="C324" s="81" t="s">
         <v>328</v>
       </c>
       <c r="D324" s="18" t="s">
@@ -25345,7 +25351,7 @@
       <c r="B325" s="38">
         <v>8</v>
       </c>
-      <c r="C325" s="18" t="s">
+      <c r="C325" s="81" t="s">
         <v>330</v>
       </c>
       <c r="D325" s="18" t="s">
@@ -25393,7 +25399,7 @@
       <c r="B326" s="38">
         <v>8</v>
       </c>
-      <c r="C326" s="18" t="s">
+      <c r="C326" s="81" t="s">
         <v>332</v>
       </c>
       <c r="D326" s="18" t="s">
@@ -25441,7 +25447,7 @@
       <c r="B327" s="38">
         <v>8</v>
       </c>
-      <c r="C327" s="18" t="s">
+      <c r="C327" s="81" t="s">
         <v>334</v>
       </c>
       <c r="D327" s="18" t="s">
@@ -25489,7 +25495,7 @@
       <c r="B328" s="38">
         <v>8</v>
       </c>
-      <c r="C328" s="18" t="s">
+      <c r="C328" s="81" t="s">
         <v>336</v>
       </c>
       <c r="D328" s="18" t="s">
@@ -25537,7 +25543,7 @@
       <c r="B329" s="38">
         <v>8</v>
       </c>
-      <c r="C329" s="18" t="s">
+      <c r="C329" s="81" t="s">
         <v>338</v>
       </c>
       <c r="D329" s="18" t="s">
@@ -25585,7 +25591,7 @@
       <c r="B330" s="38">
         <v>8</v>
       </c>
-      <c r="C330" s="18" t="s">
+      <c r="C330" s="81" t="s">
         <v>340</v>
       </c>
       <c r="D330" s="18" t="s">
@@ -25633,7 +25639,7 @@
       <c r="B331" s="38">
         <v>8</v>
       </c>
-      <c r="C331" s="18" t="s">
+      <c r="C331" s="81" t="s">
         <v>342</v>
       </c>
       <c r="D331" s="18" t="s">
@@ -25681,7 +25687,7 @@
       <c r="B332" s="38">
         <v>8</v>
       </c>
-      <c r="C332" s="18" t="s">
+      <c r="C332" s="81" t="s">
         <v>343</v>
       </c>
       <c r="D332" s="18" t="s">
@@ -25729,7 +25735,7 @@
       <c r="B333" s="38">
         <v>8</v>
       </c>
-      <c r="C333" s="18" t="s">
+      <c r="C333" s="81" t="s">
         <v>345</v>
       </c>
       <c r="D333" s="18" t="s">
@@ -25777,7 +25783,7 @@
       <c r="B334" s="38">
         <v>8</v>
       </c>
-      <c r="C334" s="18" t="s">
+      <c r="C334" s="81" t="s">
         <v>347</v>
       </c>
       <c r="D334" s="18" t="s">
@@ -25825,7 +25831,7 @@
       <c r="B335" s="38">
         <v>8</v>
       </c>
-      <c r="C335" s="18" t="s">
+      <c r="C335" s="81" t="s">
         <v>349</v>
       </c>
       <c r="D335" s="18" t="s">
@@ -25873,7 +25879,7 @@
       <c r="B336" s="38">
         <v>8</v>
       </c>
-      <c r="C336" s="18" t="s">
+      <c r="C336" s="81" t="s">
         <v>351</v>
       </c>
       <c r="D336" s="18" t="s">
@@ -25921,7 +25927,7 @@
       <c r="B337" s="38">
         <v>8</v>
       </c>
-      <c r="C337" s="18" t="s">
+      <c r="C337" s="81" t="s">
         <v>352</v>
       </c>
       <c r="D337" s="18" t="s">
@@ -26257,7 +26263,7 @@
       <c r="B344" s="38">
         <v>8</v>
       </c>
-      <c r="C344" s="18" t="s">
+      <c r="C344" s="81" t="s">
         <v>359</v>
       </c>
       <c r="D344" s="18" t="s">
@@ -26305,7 +26311,7 @@
       <c r="B345" s="38">
         <v>8</v>
       </c>
-      <c r="C345" s="18" t="s">
+      <c r="C345" s="81" t="s">
         <v>361</v>
       </c>
       <c r="D345" s="18" t="s">
@@ -26449,7 +26455,7 @@
       <c r="B348" s="38">
         <v>8</v>
       </c>
-      <c r="C348" s="18" t="s">
+      <c r="C348" s="81" t="s">
         <v>366</v>
       </c>
       <c r="D348" s="18" t="s">
@@ -26497,7 +26503,7 @@
       <c r="B349" s="38">
         <v>8</v>
       </c>
-      <c r="C349" s="18" t="s">
+      <c r="C349" s="81" t="s">
         <v>368</v>
       </c>
       <c r="D349" s="18" t="s">
@@ -26545,7 +26551,7 @@
       <c r="B350" s="38">
         <v>8</v>
       </c>
-      <c r="C350" s="18" t="s">
+      <c r="C350" s="81" t="s">
         <v>576</v>
       </c>
       <c r="D350" s="18" t="s">
@@ -26593,7 +26599,7 @@
       <c r="B351" s="38">
         <v>8</v>
       </c>
-      <c r="C351" s="18" t="s">
+      <c r="C351" s="81" t="s">
         <v>586</v>
       </c>
       <c r="D351" s="18" t="s">
@@ -26977,7 +26983,7 @@
       <c r="B359" s="38">
         <v>8</v>
       </c>
-      <c r="C359" s="18" t="s">
+      <c r="C359" s="81" t="s">
         <v>593</v>
       </c>
       <c r="D359" s="18" t="s">
@@ -27025,7 +27031,7 @@
       <c r="B360" s="38">
         <v>8</v>
       </c>
-      <c r="C360" s="18" t="s">
+      <c r="C360" s="81" t="s">
         <v>605</v>
       </c>
       <c r="D360" s="18" t="s">
@@ -27073,7 +27079,7 @@
       <c r="B361" s="38">
         <v>8</v>
       </c>
-      <c r="C361" s="18" t="s">
+      <c r="C361" s="81" t="s">
         <v>606</v>
       </c>
       <c r="D361" s="18" t="s">
@@ -27121,7 +27127,7 @@
       <c r="B362" s="38">
         <v>8</v>
       </c>
-      <c r="C362" s="18" t="s">
+      <c r="C362" s="81" t="s">
         <v>607</v>
       </c>
       <c r="D362" s="18" t="s">
@@ -27169,7 +27175,7 @@
       <c r="B363" s="38">
         <v>8</v>
       </c>
-      <c r="C363" s="18" t="s">
+      <c r="C363" s="81" t="s">
         <v>608</v>
       </c>
       <c r="D363" s="18" t="s">
@@ -27217,7 +27223,7 @@
       <c r="B364" s="38">
         <v>8</v>
       </c>
-      <c r="C364" s="18" t="s">
+      <c r="C364" s="81" t="s">
         <v>609</v>
       </c>
       <c r="D364" s="18" t="s">
@@ -27265,7 +27271,7 @@
       <c r="B365" s="38">
         <v>8</v>
       </c>
-      <c r="C365" s="18" t="s">
+      <c r="C365" s="81" t="s">
         <v>610</v>
       </c>
       <c r="D365" s="18" t="s">
@@ -27313,7 +27319,7 @@
       <c r="B366" s="38">
         <v>8</v>
       </c>
-      <c r="C366" s="18" t="s">
+      <c r="C366" s="81" t="s">
         <v>611</v>
       </c>
       <c r="D366" s="18" t="s">
@@ -27361,7 +27367,7 @@
       <c r="B367" s="38">
         <v>8</v>
       </c>
-      <c r="C367" s="18" t="s">
+      <c r="C367" s="81" t="s">
         <v>612</v>
       </c>
       <c r="D367" s="18" t="s">
@@ -27409,7 +27415,7 @@
       <c r="B368" s="38">
         <v>8</v>
       </c>
-      <c r="C368" s="18" t="s">
+      <c r="C368" s="81" t="s">
         <v>645</v>
       </c>
       <c r="D368" s="18" t="s">
@@ -27457,7 +27463,7 @@
       <c r="B369" s="38">
         <v>8</v>
       </c>
-      <c r="C369" s="18" t="s">
+      <c r="C369" s="81" t="s">
         <v>1166</v>
       </c>
       <c r="D369" s="18" t="s">
@@ -27505,7 +27511,7 @@
       <c r="B370" s="38">
         <v>8</v>
       </c>
-      <c r="C370" s="18" t="s">
+      <c r="C370" s="81" t="s">
         <v>1244</v>
       </c>
       <c r="D370" s="18" t="s">
@@ -27601,7 +27607,7 @@
       <c r="B372" s="38">
         <v>8</v>
       </c>
-      <c r="C372" s="18" t="s">
+      <c r="C372" s="81" t="s">
         <v>583</v>
       </c>
       <c r="D372" s="18" t="s">
@@ -27649,7 +27655,7 @@
       <c r="B373" s="38">
         <v>8</v>
       </c>
-      <c r="C373" s="18" t="s">
+      <c r="C373" s="81" t="s">
         <v>1246</v>
       </c>
       <c r="D373" s="18" t="s">
@@ -27745,7 +27751,7 @@
       <c r="B375" s="38">
         <v>8</v>
       </c>
-      <c r="C375" s="18" t="s">
+      <c r="C375" s="81" t="s">
         <v>648</v>
       </c>
       <c r="D375" s="18" t="s">
@@ -28177,7 +28183,7 @@
       <c r="B384" s="38">
         <v>8</v>
       </c>
-      <c r="C384" s="18" t="s">
+      <c r="C384" s="81" t="s">
         <v>1173</v>
       </c>
       <c r="D384" s="18" t="s">
@@ -28225,7 +28231,7 @@
       <c r="B385" s="38">
         <v>8</v>
       </c>
-      <c r="C385" s="18" t="s">
+      <c r="C385" s="81" t="s">
         <v>1174</v>
       </c>
       <c r="D385" s="18" t="s">
@@ -28273,7 +28279,7 @@
       <c r="B386" s="38">
         <v>8</v>
       </c>
-      <c r="C386" s="18" t="s">
+      <c r="C386" s="81" t="s">
         <v>1175</v>
       </c>
       <c r="D386" s="18" t="s">
@@ -28321,7 +28327,7 @@
       <c r="B387" s="38">
         <v>8</v>
       </c>
-      <c r="C387" s="18" t="s">
+      <c r="C387" s="81" t="s">
         <v>1176</v>
       </c>
       <c r="D387" s="18" t="s">
@@ -28369,7 +28375,7 @@
       <c r="B388" s="38">
         <v>8</v>
       </c>
-      <c r="C388" s="18" t="s">
+      <c r="C388" s="81" t="s">
         <v>1177</v>
       </c>
       <c r="D388" s="18" t="s">
@@ -28417,7 +28423,7 @@
       <c r="B389" s="38">
         <v>8</v>
       </c>
-      <c r="C389" s="18" t="s">
+      <c r="C389" s="81" t="s">
         <v>1178</v>
       </c>
       <c r="D389" s="18" t="s">
@@ -28465,7 +28471,7 @@
       <c r="B390" s="38">
         <v>8</v>
       </c>
-      <c r="C390" s="18" t="s">
+      <c r="C390" s="81" t="s">
         <v>1179</v>
       </c>
       <c r="D390" s="18" t="s">
@@ -28513,7 +28519,7 @@
       <c r="B391" s="38">
         <v>8</v>
       </c>
-      <c r="C391" s="18" t="s">
+      <c r="C391" s="81" t="s">
         <v>1180</v>
       </c>
       <c r="D391" s="18" t="s">
@@ -28561,7 +28567,7 @@
       <c r="B392" s="38">
         <v>8</v>
       </c>
-      <c r="C392" s="18" t="s">
+      <c r="C392" s="81" t="s">
         <v>1181</v>
       </c>
       <c r="D392" s="18" t="s">
@@ -28609,7 +28615,7 @@
       <c r="B393" s="38">
         <v>8</v>
       </c>
-      <c r="C393" s="18" t="s">
+      <c r="C393" s="81" t="s">
         <v>1182</v>
       </c>
       <c r="D393" s="18" t="s">
@@ -28657,7 +28663,7 @@
       <c r="B394" s="38">
         <v>8</v>
       </c>
-      <c r="C394" s="18" t="s">
+      <c r="C394" s="81" t="s">
         <v>1183</v>
       </c>
       <c r="D394" s="18" t="s">
@@ -28753,7 +28759,7 @@
       <c r="B396" s="38">
         <v>8</v>
       </c>
-      <c r="C396" s="18" t="s">
+      <c r="C396" s="81" t="s">
         <v>1184</v>
       </c>
       <c r="D396" s="18" t="s">
@@ -28801,7 +28807,7 @@
       <c r="B397" s="38">
         <v>8</v>
       </c>
-      <c r="C397" s="18" t="s">
+      <c r="C397" s="81" t="s">
         <v>1185</v>
       </c>
       <c r="D397" s="18" t="s">
@@ -28849,7 +28855,7 @@
       <c r="B398" s="38">
         <v>8</v>
       </c>
-      <c r="C398" s="18" t="s">
+      <c r="C398" s="81" t="s">
         <v>1186</v>
       </c>
       <c r="D398" s="18" t="s">
@@ -28897,7 +28903,7 @@
       <c r="B399" s="38">
         <v>8</v>
       </c>
-      <c r="C399" s="18" t="s">
+      <c r="C399" s="81" t="s">
         <v>1187</v>
       </c>
       <c r="D399" s="18" t="s">
@@ -28945,7 +28951,7 @@
       <c r="B400" s="38">
         <v>8</v>
       </c>
-      <c r="C400" s="18" t="s">
+      <c r="C400" s="81" t="s">
         <v>1188</v>
       </c>
       <c r="D400" s="18" t="s">
@@ -28993,7 +28999,7 @@
       <c r="B401" s="38">
         <v>8</v>
       </c>
-      <c r="C401" s="18" t="s">
+      <c r="C401" s="81" t="s">
         <v>1193</v>
       </c>
       <c r="D401" s="18" t="s">
@@ -29041,7 +29047,7 @@
       <c r="B402" s="38">
         <v>8</v>
       </c>
-      <c r="C402" s="18" t="s">
+      <c r="C402" s="81" t="s">
         <v>1248</v>
       </c>
       <c r="D402" s="18" t="s">
@@ -29089,7 +29095,7 @@
       <c r="B403" s="38">
         <v>8</v>
       </c>
-      <c r="C403" s="18" t="s">
+      <c r="C403" s="81" t="s">
         <v>1249</v>
       </c>
       <c r="D403" s="18" t="s">
@@ -29137,7 +29143,7 @@
       <c r="B404" s="38">
         <v>8</v>
       </c>
-      <c r="C404" s="18" t="s">
+      <c r="C404" s="81" t="s">
         <v>1250</v>
       </c>
       <c r="D404" s="18" t="s">
@@ -30097,7 +30103,7 @@
       <c r="B424" s="38">
         <v>8</v>
       </c>
-      <c r="C424" s="18" t="s">
+      <c r="C424" s="81" t="s">
         <v>370</v>
       </c>
       <c r="D424" s="18" t="s">
@@ -30628,7 +30634,7 @@
       <c r="C435" s="18" t="s">
         <v>1754</v>
       </c>
-      <c r="D435" s="18" t="s">
+      <c r="D435" s="79" t="s">
         <v>1753</v>
       </c>
       <c r="E435" s="12" t="s">
@@ -30913,7 +30919,7 @@
       <c r="B441" s="38">
         <v>8</v>
       </c>
-      <c r="C441" s="18" t="s">
+      <c r="C441" s="81" t="s">
         <v>1253</v>
       </c>
       <c r="D441" s="18" t="s">
@@ -32545,7 +32551,7 @@
       <c r="B475" s="38">
         <v>2</v>
       </c>
-      <c r="C475" s="18" t="s">
+      <c r="C475" s="81" t="s">
         <v>814</v>
       </c>
       <c r="D475" s="18" t="s">
@@ -32593,7 +32599,7 @@
       <c r="B476" s="38">
         <v>2</v>
       </c>
-      <c r="C476" s="18" t="s">
+      <c r="C476" s="81" t="s">
         <v>816</v>
       </c>
       <c r="D476" s="18" t="s">
@@ -32641,7 +32647,7 @@
       <c r="B477" s="38">
         <v>2</v>
       </c>
-      <c r="C477" s="18" t="s">
+      <c r="C477" s="81" t="s">
         <v>783</v>
       </c>
       <c r="D477" s="18" t="s">
@@ -32689,7 +32695,7 @@
       <c r="B478" s="38">
         <v>2</v>
       </c>
-      <c r="C478" s="18" t="s">
+      <c r="C478" s="81" t="s">
         <v>770</v>
       </c>
       <c r="D478" s="18" t="s">
@@ -32737,7 +32743,7 @@
       <c r="B479" s="38">
         <v>2</v>
       </c>
-      <c r="C479" s="18" t="s">
+      <c r="C479" s="81" t="s">
         <v>820</v>
       </c>
       <c r="D479" s="18" t="s">
@@ -32833,7 +32839,7 @@
       <c r="B481" s="38">
         <v>2</v>
       </c>
-      <c r="C481" s="18" t="s">
+      <c r="C481" s="81" t="s">
         <v>769</v>
       </c>
       <c r="D481" s="18" t="s">
@@ -32881,7 +32887,7 @@
       <c r="B482" s="38">
         <v>2</v>
       </c>
-      <c r="C482" s="18" t="s">
+      <c r="C482" s="81" t="s">
         <v>773</v>
       </c>
       <c r="D482" s="18" t="s">
@@ -32929,7 +32935,7 @@
       <c r="B483" s="38">
         <v>2</v>
       </c>
-      <c r="C483" s="18" t="s">
+      <c r="C483" s="81" t="s">
         <v>789</v>
       </c>
       <c r="D483" s="18" t="s">
@@ -32977,7 +32983,7 @@
       <c r="B484" s="38">
         <v>2</v>
       </c>
-      <c r="C484" s="18" t="s">
+      <c r="C484" s="81" t="s">
         <v>774</v>
       </c>
       <c r="D484" s="18" t="s">
@@ -33025,7 +33031,7 @@
       <c r="B485" s="38">
         <v>2</v>
       </c>
-      <c r="C485" s="18" t="s">
+      <c r="C485" s="81" t="s">
         <v>826</v>
       </c>
       <c r="D485" s="18" t="s">
@@ -33073,7 +33079,7 @@
       <c r="B486" s="38">
         <v>2</v>
       </c>
-      <c r="C486" s="18" t="s">
+      <c r="C486" s="81" t="s">
         <v>828</v>
       </c>
       <c r="D486" s="18" t="s">
@@ -33121,7 +33127,7 @@
       <c r="B487" s="38">
         <v>2</v>
       </c>
-      <c r="C487" s="18" t="s">
+      <c r="C487" s="81" t="s">
         <v>786</v>
       </c>
       <c r="D487" s="18" t="s">
@@ -33313,7 +33319,7 @@
       <c r="B491" s="38">
         <v>2</v>
       </c>
-      <c r="C491" s="18" t="s">
+      <c r="C491" s="81" t="s">
         <v>834</v>
       </c>
       <c r="D491" s="18" t="s">
@@ -33361,7 +33367,7 @@
       <c r="B492" s="38">
         <v>2</v>
       </c>
-      <c r="C492" s="18" t="s">
+      <c r="C492" s="81" t="s">
         <v>836</v>
       </c>
       <c r="D492" s="18" t="s">
@@ -33649,7 +33655,7 @@
       <c r="B498" s="38">
         <v>2</v>
       </c>
-      <c r="C498" s="18" t="s">
+      <c r="C498" s="81" t="s">
         <v>847</v>
       </c>
       <c r="D498" s="18" t="s">
@@ -33697,7 +33703,7 @@
       <c r="B499" s="38">
         <v>2</v>
       </c>
-      <c r="C499" s="18" t="s">
+      <c r="C499" s="81" t="s">
         <v>849</v>
       </c>
       <c r="D499" s="18" t="s">
@@ -33745,7 +33751,7 @@
       <c r="B500" s="38">
         <v>2</v>
       </c>
-      <c r="C500" s="18" t="s">
+      <c r="C500" s="81" t="s">
         <v>777</v>
       </c>
       <c r="D500" s="18" t="s">
@@ -33793,7 +33799,7 @@
       <c r="B501" s="38">
         <v>2</v>
       </c>
-      <c r="C501" s="18" t="s">
+      <c r="C501" s="81" t="s">
         <v>791</v>
       </c>
       <c r="D501" s="18" t="s">
@@ -33841,7 +33847,7 @@
       <c r="B502" s="38">
         <v>2</v>
       </c>
-      <c r="C502" s="18" t="s">
+      <c r="C502" s="81" t="s">
         <v>852</v>
       </c>
       <c r="D502" s="18" t="s">
@@ -33889,7 +33895,7 @@
       <c r="B503" s="38">
         <v>2</v>
       </c>
-      <c r="C503" s="18" t="s">
+      <c r="C503" s="81" t="s">
         <v>778</v>
       </c>
       <c r="D503" s="18" t="s">
@@ -33937,7 +33943,7 @@
       <c r="B504" s="38">
         <v>2</v>
       </c>
-      <c r="C504" s="18" t="s">
+      <c r="C504" s="81" t="s">
         <v>779</v>
       </c>
       <c r="D504" s="18" t="s">
@@ -34225,7 +34231,7 @@
       <c r="B510" s="38">
         <v>2</v>
       </c>
-      <c r="C510" s="18" t="s">
+      <c r="C510" s="81" t="s">
         <v>860</v>
       </c>
       <c r="D510" s="18" t="s">
@@ -34273,7 +34279,7 @@
       <c r="B511" s="38">
         <v>2</v>
       </c>
-      <c r="C511" s="18" t="s">
+      <c r="C511" s="81" t="s">
         <v>862</v>
       </c>
       <c r="D511" s="18" t="s">
@@ -34321,7 +34327,7 @@
       <c r="B512" s="38">
         <v>2</v>
       </c>
-      <c r="C512" s="18" t="s">
+      <c r="C512" s="81" t="s">
         <v>787</v>
       </c>
       <c r="D512" s="18" t="s">
@@ -34369,7 +34375,7 @@
       <c r="B513" s="38">
         <v>2</v>
       </c>
-      <c r="C513" s="18" t="s">
+      <c r="C513" s="81" t="s">
         <v>788</v>
       </c>
       <c r="D513" s="18" t="s">
@@ -34513,7 +34519,7 @@
       <c r="B516" s="38">
         <v>2</v>
       </c>
-      <c r="C516" s="18" t="s">
+      <c r="C516" s="81" t="s">
         <v>813</v>
       </c>
       <c r="D516" s="18" t="s">
@@ -34609,7 +34615,7 @@
       <c r="B518" s="38">
         <v>2</v>
       </c>
-      <c r="C518" s="18" t="s">
+      <c r="C518" s="81" t="s">
         <v>1009</v>
       </c>
       <c r="D518" s="18" t="s">
@@ -35137,7 +35143,7 @@
       <c r="B529" s="38">
         <v>2</v>
       </c>
-      <c r="C529" s="18" t="s">
+      <c r="C529" s="81" t="s">
         <v>868</v>
       </c>
       <c r="D529" s="18" t="s">
@@ -35185,7 +35191,7 @@
       <c r="B530" s="38">
         <v>2</v>
       </c>
-      <c r="C530" s="18" t="s">
+      <c r="C530" s="81" t="s">
         <v>870</v>
       </c>
       <c r="D530" s="18" t="s">
@@ -35233,7 +35239,7 @@
       <c r="B531" s="38">
         <v>2</v>
       </c>
-      <c r="C531" s="18" t="s">
+      <c r="C531" s="81" t="s">
         <v>872</v>
       </c>
       <c r="D531" s="18" t="s">
@@ -35281,7 +35287,7 @@
       <c r="B532" s="38">
         <v>2</v>
       </c>
-      <c r="C532" s="18" t="s">
+      <c r="C532" s="81" t="s">
         <v>874</v>
       </c>
       <c r="D532" s="18" t="s">
@@ -35329,7 +35335,7 @@
       <c r="B533" s="38">
         <v>2</v>
       </c>
-      <c r="C533" s="18" t="s">
+      <c r="C533" s="81" t="s">
         <v>876</v>
       </c>
       <c r="D533" s="18" t="s">
@@ -35377,7 +35383,7 @@
       <c r="B534" s="38">
         <v>2</v>
       </c>
-      <c r="C534" s="18" t="s">
+      <c r="C534" s="81" t="s">
         <v>878</v>
       </c>
       <c r="D534" s="18" t="s">
@@ -35425,7 +35431,7 @@
       <c r="B535" s="38">
         <v>2</v>
       </c>
-      <c r="C535" s="18" t="s">
+      <c r="C535" s="81" t="s">
         <v>767</v>
       </c>
       <c r="D535" s="18" t="s">
@@ -35473,7 +35479,7 @@
       <c r="B536" s="38">
         <v>2</v>
       </c>
-      <c r="C536" s="18" t="s">
+      <c r="C536" s="81" t="s">
         <v>879</v>
       </c>
       <c r="D536" s="18" t="s">
@@ -35521,7 +35527,7 @@
       <c r="B537" s="38">
         <v>2</v>
       </c>
-      <c r="C537" s="18" t="s">
+      <c r="C537" s="81" t="s">
         <v>881</v>
       </c>
       <c r="D537" s="18" t="s">
@@ -35569,7 +35575,7 @@
       <c r="B538" s="38">
         <v>2</v>
       </c>
-      <c r="C538" s="18" t="s">
+      <c r="C538" s="81" t="s">
         <v>804</v>
       </c>
       <c r="D538" s="18" t="s">
@@ -35617,7 +35623,7 @@
       <c r="B539" s="38">
         <v>2</v>
       </c>
-      <c r="C539" s="18" t="s">
+      <c r="C539" s="81" t="s">
         <v>766</v>
       </c>
       <c r="D539" s="18" t="s">
@@ -35665,7 +35671,7 @@
       <c r="B540" s="38">
         <v>2</v>
       </c>
-      <c r="C540" s="18" t="s">
+      <c r="C540" s="81" t="s">
         <v>884</v>
       </c>
       <c r="D540" s="18" t="s">
@@ -35713,7 +35719,7 @@
       <c r="B541" s="38">
         <v>2</v>
       </c>
-      <c r="C541" s="18" t="s">
+      <c r="C541" s="81" t="s">
         <v>885</v>
       </c>
       <c r="D541" s="18" t="s">
@@ -35761,7 +35767,7 @@
       <c r="B542" s="38">
         <v>2</v>
       </c>
-      <c r="C542" s="18" t="s">
+      <c r="C542" s="81" t="s">
         <v>886</v>
       </c>
       <c r="D542" s="18" t="s">
@@ -35809,7 +35815,7 @@
       <c r="B543" s="38">
         <v>2</v>
       </c>
-      <c r="C543" s="18" t="s">
+      <c r="C543" s="81" t="s">
         <v>888</v>
       </c>
       <c r="D543" s="18" t="s">
@@ -35953,7 +35959,7 @@
       <c r="B546" s="38">
         <v>2</v>
       </c>
-      <c r="C546" s="18" t="s">
+      <c r="C546" s="81" t="s">
         <v>892</v>
       </c>
       <c r="D546" s="18" t="s">
@@ -36001,7 +36007,7 @@
       <c r="B547" s="38">
         <v>2</v>
       </c>
-      <c r="C547" s="18" t="s">
+      <c r="C547" s="81" t="s">
         <v>809</v>
       </c>
       <c r="D547" s="18" t="s">
@@ -36049,7 +36055,7 @@
       <c r="B548" s="38">
         <v>2</v>
       </c>
-      <c r="C548" s="18" t="s">
+      <c r="C548" s="81" t="s">
         <v>894</v>
       </c>
       <c r="D548" s="18" t="s">
@@ -36097,7 +36103,7 @@
       <c r="B549" s="38">
         <v>2</v>
       </c>
-      <c r="C549" s="18" t="s">
+      <c r="C549" s="81" t="s">
         <v>812</v>
       </c>
       <c r="D549" s="18" t="s">
@@ -36145,7 +36151,7 @@
       <c r="B550" s="38">
         <v>2</v>
       </c>
-      <c r="C550" s="18" t="s">
+      <c r="C550" s="81" t="s">
         <v>897</v>
       </c>
       <c r="D550" s="18" t="s">
@@ -36289,7 +36295,7 @@
       <c r="B553" s="38">
         <v>2</v>
       </c>
-      <c r="C553" s="18" t="s">
+      <c r="C553" s="81" t="s">
         <v>900</v>
       </c>
       <c r="D553" s="18" t="s">
@@ -36337,7 +36343,7 @@
       <c r="B554" s="38">
         <v>2</v>
       </c>
-      <c r="C554" s="18" t="s">
+      <c r="C554" s="81" t="s">
         <v>902</v>
       </c>
       <c r="D554" s="18" t="s">
@@ -36481,7 +36487,7 @@
       <c r="B557" s="38">
         <v>2</v>
       </c>
-      <c r="C557" s="18" t="s">
+      <c r="C557" s="81" t="s">
         <v>810</v>
       </c>
       <c r="D557" s="18" t="s">
@@ -36529,7 +36535,7 @@
       <c r="B558" s="38">
         <v>2</v>
       </c>
-      <c r="C558" s="18" t="s">
+      <c r="C558" s="81" t="s">
         <v>811</v>
       </c>
       <c r="D558" s="18" t="s">
@@ -36577,7 +36583,7 @@
       <c r="B559" s="38">
         <v>2</v>
       </c>
-      <c r="C559" s="18" t="s">
+      <c r="C559" s="81" t="s">
         <v>798</v>
       </c>
       <c r="D559" s="18" t="s">
@@ -36625,7 +36631,7 @@
       <c r="B560" s="38">
         <v>2</v>
       </c>
-      <c r="C560" s="18" t="s">
+      <c r="C560" s="81" t="s">
         <v>800</v>
       </c>
       <c r="D560" s="18" t="s">
@@ -36673,7 +36679,7 @@
       <c r="B561" s="38">
         <v>2</v>
       </c>
-      <c r="C561" s="18" t="s">
+      <c r="C561" s="81" t="s">
         <v>801</v>
       </c>
       <c r="D561" s="18" t="s">
@@ -36721,7 +36727,7 @@
       <c r="B562" s="38">
         <v>2</v>
       </c>
-      <c r="C562" s="18" t="s">
+      <c r="C562" s="81" t="s">
         <v>802</v>
       </c>
       <c r="D562" s="18" t="s">
@@ -36769,7 +36775,7 @@
       <c r="B563" s="38">
         <v>2</v>
       </c>
-      <c r="C563" s="18" t="s">
+      <c r="C563" s="81" t="s">
         <v>803</v>
       </c>
       <c r="D563" s="18" t="s">
@@ -36817,7 +36823,7 @@
       <c r="B564" s="38">
         <v>4</v>
       </c>
-      <c r="C564" s="18" t="s">
+      <c r="C564" s="81" t="s">
         <v>707</v>
       </c>
       <c r="D564" s="18" t="s">
@@ -36865,7 +36871,7 @@
       <c r="B565" s="38">
         <v>4</v>
       </c>
-      <c r="C565" s="18" t="s">
+      <c r="C565" s="81" t="s">
         <v>709</v>
       </c>
       <c r="D565" s="18" t="s">
@@ -36913,7 +36919,7 @@
       <c r="B566" s="38">
         <v>4</v>
       </c>
-      <c r="C566" s="18" t="s">
+      <c r="C566" s="81" t="s">
         <v>711</v>
       </c>
       <c r="D566" s="18" t="s">
@@ -36961,7 +36967,7 @@
       <c r="B567" s="38">
         <v>4</v>
       </c>
-      <c r="C567" s="18" t="s">
+      <c r="C567" s="81" t="s">
         <v>713</v>
       </c>
       <c r="D567" s="18" t="s">
@@ -37009,7 +37015,7 @@
       <c r="B568" s="38">
         <v>4</v>
       </c>
-      <c r="C568" s="18" t="s">
+      <c r="C568" s="81" t="s">
         <v>715</v>
       </c>
       <c r="D568" s="18" t="s">
@@ -37105,7 +37111,7 @@
       <c r="B570" s="38">
         <v>4</v>
       </c>
-      <c r="C570" s="18" t="s">
+      <c r="C570" s="81" t="s">
         <v>718</v>
       </c>
       <c r="D570" s="18" t="s">
@@ -37153,7 +37159,7 @@
       <c r="B571" s="38">
         <v>4</v>
       </c>
-      <c r="C571" s="18" t="s">
+      <c r="C571" s="81" t="s">
         <v>720</v>
       </c>
       <c r="D571" s="18" t="s">
@@ -37201,7 +37207,7 @@
       <c r="B572" s="38">
         <v>4</v>
       </c>
-      <c r="C572" s="18" t="s">
+      <c r="C572" s="81" t="s">
         <v>722</v>
       </c>
       <c r="D572" s="18" t="s">
@@ -37249,7 +37255,7 @@
       <c r="B573" s="38">
         <v>4</v>
       </c>
-      <c r="C573" s="18" t="s">
+      <c r="C573" s="81" t="s">
         <v>723</v>
       </c>
       <c r="D573" s="18" t="s">
@@ -37297,7 +37303,7 @@
       <c r="B574" s="38">
         <v>4</v>
       </c>
-      <c r="C574" s="18" t="s">
+      <c r="C574" s="81" t="s">
         <v>725</v>
       </c>
       <c r="D574" s="18" t="s">
@@ -37345,7 +37351,7 @@
       <c r="B575" s="38">
         <v>4</v>
       </c>
-      <c r="C575" s="18" t="s">
+      <c r="C575" s="81" t="s">
         <v>727</v>
       </c>
       <c r="D575" s="18" t="s">
@@ -37393,7 +37399,7 @@
       <c r="B576" s="38">
         <v>4</v>
       </c>
-      <c r="C576" s="18" t="s">
+      <c r="C576" s="81" t="s">
         <v>729</v>
       </c>
       <c r="D576" s="18" t="s">
@@ -37441,7 +37447,7 @@
       <c r="B577" s="38">
         <v>4</v>
       </c>
-      <c r="C577" s="18" t="s">
+      <c r="C577" s="81" t="s">
         <v>731</v>
       </c>
       <c r="D577" s="18" t="s">
@@ -37537,7 +37543,7 @@
       <c r="B579" s="38">
         <v>2</v>
       </c>
-      <c r="C579" s="18" t="s">
+      <c r="C579" s="81" t="s">
         <v>792</v>
       </c>
       <c r="D579" s="18" t="s">
@@ -37585,7 +37591,7 @@
       <c r="B580" s="38">
         <v>4</v>
       </c>
-      <c r="C580" s="18" t="s">
+      <c r="C580" s="81" t="s">
         <v>793</v>
       </c>
       <c r="D580" s="18" t="s">
@@ -37681,7 +37687,7 @@
       <c r="B582" s="38">
         <v>4</v>
       </c>
-      <c r="C582" s="18" t="s">
+      <c r="C582" s="81" t="s">
         <v>916</v>
       </c>
       <c r="D582" s="18" t="s">
@@ -37729,7 +37735,7 @@
       <c r="B583" s="38">
         <v>4</v>
       </c>
-      <c r="C583" s="18" t="s">
+      <c r="C583" s="81" t="s">
         <v>918</v>
       </c>
       <c r="D583" s="18" t="s">
@@ -37777,7 +37783,7 @@
       <c r="B584" s="38">
         <v>4</v>
       </c>
-      <c r="C584" s="18" t="s">
+      <c r="C584" s="81" t="s">
         <v>920</v>
       </c>
       <c r="D584" s="18" t="s">
@@ -37825,7 +37831,7 @@
       <c r="B585" s="38">
         <v>4</v>
       </c>
-      <c r="C585" s="18" t="s">
+      <c r="C585" s="81" t="s">
         <v>922</v>
       </c>
       <c r="D585" s="18" t="s">
@@ -37873,7 +37879,7 @@
       <c r="B586" s="38">
         <v>4</v>
       </c>
-      <c r="C586" s="18" t="s">
+      <c r="C586" s="81" t="s">
         <v>924</v>
       </c>
       <c r="D586" s="18" t="s">
@@ -37921,7 +37927,7 @@
       <c r="B587" s="38">
         <v>4</v>
       </c>
-      <c r="C587" s="18" t="s">
+      <c r="C587" s="81" t="s">
         <v>926</v>
       </c>
       <c r="D587" s="18" t="s">
@@ -37969,7 +37975,7 @@
       <c r="B588" s="38">
         <v>4</v>
       </c>
-      <c r="C588" s="18" t="s">
+      <c r="C588" s="81" t="s">
         <v>928</v>
       </c>
       <c r="D588" s="18" t="s">
@@ -38017,7 +38023,7 @@
       <c r="B589" s="38">
         <v>4</v>
       </c>
-      <c r="C589" s="18" t="s">
+      <c r="C589" s="81" t="s">
         <v>930</v>
       </c>
       <c r="D589" s="18" t="s">
@@ -38065,7 +38071,7 @@
       <c r="B590" s="38">
         <v>4</v>
       </c>
-      <c r="C590" s="18" t="s">
+      <c r="C590" s="81" t="s">
         <v>932</v>
       </c>
       <c r="D590" s="18" t="s">
@@ -38113,7 +38119,7 @@
       <c r="B591" s="38">
         <v>4</v>
       </c>
-      <c r="C591" s="18" t="s">
+      <c r="C591" s="81" t="s">
         <v>934</v>
       </c>
       <c r="D591" s="18" t="s">
@@ -38161,7 +38167,7 @@
       <c r="B592" s="38">
         <v>4</v>
       </c>
-      <c r="C592" s="18" t="s">
+      <c r="C592" s="81" t="s">
         <v>936</v>
       </c>
       <c r="D592" s="18" t="s">
@@ -38209,7 +38215,7 @@
       <c r="B593" s="38">
         <v>4</v>
       </c>
-      <c r="C593" s="18" t="s">
+      <c r="C593" s="81" t="s">
         <v>938</v>
       </c>
       <c r="D593" s="18" t="s">
@@ -38257,7 +38263,7 @@
       <c r="B594" s="38">
         <v>4</v>
       </c>
-      <c r="C594" s="18" t="s">
+      <c r="C594" s="81" t="s">
         <v>940</v>
       </c>
       <c r="D594" s="18" t="s">
@@ -38305,7 +38311,7 @@
       <c r="B595" s="38">
         <v>4</v>
       </c>
-      <c r="C595" s="18" t="s">
+      <c r="C595" s="81" t="s">
         <v>942</v>
       </c>
       <c r="D595" s="18" t="s">
@@ -38353,7 +38359,7 @@
       <c r="B596" s="38">
         <v>4</v>
       </c>
-      <c r="C596" s="18" t="s">
+      <c r="C596" s="81" t="s">
         <v>944</v>
       </c>
       <c r="D596" s="18" t="s">
@@ -38401,7 +38407,7 @@
       <c r="B597" s="38">
         <v>4</v>
       </c>
-      <c r="C597" s="18" t="s">
+      <c r="C597" s="81" t="s">
         <v>946</v>
       </c>
       <c r="D597" s="18" t="s">
@@ -38449,7 +38455,7 @@
       <c r="B598" s="38">
         <v>4</v>
       </c>
-      <c r="C598" s="18" t="s">
+      <c r="C598" s="81" t="s">
         <v>948</v>
       </c>
       <c r="D598" s="18" t="s">
@@ -38497,7 +38503,7 @@
       <c r="B599" s="38">
         <v>4</v>
       </c>
-      <c r="C599" s="18" t="s">
+      <c r="C599" s="81" t="s">
         <v>950</v>
       </c>
       <c r="D599" s="18" t="s">
@@ -38545,7 +38551,7 @@
       <c r="B600" s="38">
         <v>4</v>
       </c>
-      <c r="C600" s="18" t="s">
+      <c r="C600" s="81" t="s">
         <v>951</v>
       </c>
       <c r="D600" s="18" t="s">
@@ -38593,7 +38599,7 @@
       <c r="B601" s="38">
         <v>4</v>
       </c>
-      <c r="C601" s="18" t="s">
+      <c r="C601" s="81" t="s">
         <v>953</v>
       </c>
       <c r="D601" s="18" t="s">
@@ -38641,7 +38647,7 @@
       <c r="B602" s="38">
         <v>4</v>
       </c>
-      <c r="C602" s="18" t="s">
+      <c r="C602" s="81" t="s">
         <v>955</v>
       </c>
       <c r="D602" s="18" t="s">
@@ -38689,7 +38695,7 @@
       <c r="B603" s="38">
         <v>4</v>
       </c>
-      <c r="C603" s="18" t="s">
+      <c r="C603" s="81" t="s">
         <v>957</v>
       </c>
       <c r="D603" s="18" t="s">
@@ -38737,7 +38743,7 @@
       <c r="B604" s="38">
         <v>4</v>
       </c>
-      <c r="C604" s="18" t="s">
+      <c r="C604" s="81" t="s">
         <v>958</v>
       </c>
       <c r="D604" s="18" t="s">
@@ -38785,7 +38791,7 @@
       <c r="B605" s="38">
         <v>4</v>
       </c>
-      <c r="C605" s="18" t="s">
+      <c r="C605" s="81" t="s">
         <v>960</v>
       </c>
       <c r="D605" s="18" t="s">
@@ -38833,7 +38839,7 @@
       <c r="B606" s="38">
         <v>4</v>
       </c>
-      <c r="C606" s="18" t="s">
+      <c r="C606" s="81" t="s">
         <v>962</v>
       </c>
       <c r="D606" s="18" t="s">
@@ -38881,7 +38887,7 @@
       <c r="B607" s="38">
         <v>4</v>
       </c>
-      <c r="C607" s="18" t="s">
+      <c r="C607" s="81" t="s">
         <v>964</v>
       </c>
       <c r="D607" s="18" t="s">
@@ -38929,7 +38935,7 @@
       <c r="B608" s="38">
         <v>4</v>
       </c>
-      <c r="C608" s="18" t="s">
+      <c r="C608" s="81" t="s">
         <v>966</v>
       </c>
       <c r="D608" s="18" t="s">
@@ -38977,7 +38983,7 @@
       <c r="B609" s="38">
         <v>4</v>
       </c>
-      <c r="C609" s="18" t="s">
+      <c r="C609" s="81" t="s">
         <v>968</v>
       </c>
       <c r="D609" s="18" t="s">
@@ -42673,7 +42679,7 @@
       <c r="B686" s="38">
         <v>8</v>
       </c>
-      <c r="C686" s="18" t="s">
+      <c r="C686" s="81" t="s">
         <v>463</v>
       </c>
       <c r="D686" s="18" t="s">
@@ -42721,7 +42727,7 @@
       <c r="B687" s="38">
         <v>8</v>
       </c>
-      <c r="C687" s="18" t="s">
+      <c r="C687" s="81" t="s">
         <v>268</v>
       </c>
       <c r="D687" s="18" t="s">
@@ -42817,7 +42823,7 @@
       <c r="B689" s="38">
         <v>8</v>
       </c>
-      <c r="C689" s="18" t="s">
+      <c r="C689" s="81" t="s">
         <v>457</v>
       </c>
       <c r="D689" s="18" t="s">
@@ -43153,7 +43159,7 @@
       <c r="B696" s="38">
         <v>8</v>
       </c>
-      <c r="C696" s="18" t="s">
+      <c r="C696" s="81" t="s">
         <v>464</v>
       </c>
       <c r="D696" s="18" t="s">
@@ -43201,7 +43207,7 @@
       <c r="B697" s="38">
         <v>8</v>
       </c>
-      <c r="C697" s="18" t="s">
+      <c r="C697" s="81" t="s">
         <v>466</v>
       </c>
       <c r="D697" s="18" t="s">
@@ -43489,7 +43495,7 @@
       <c r="B703" s="38">
         <v>8</v>
       </c>
-      <c r="C703" s="18" t="s">
+      <c r="C703" s="81" t="s">
         <v>1257</v>
       </c>
       <c r="D703" s="18" t="s">
@@ -49416,10 +49422,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="78"/>
       <c r="C1" s="6" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
2021-07-01:1150: generated new test-set
</commit_message>
<xml_diff>
--- a/1.0.4-matrix-1.3-rc/matrix/Validatiematrix_v1.3-rc.xlsx
+++ b/1.0.4-matrix-1.3-rc/matrix/Validatiematrix_v1.3-rc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4-matrix-1.3-rc\matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C245252-FB8A-426A-867F-5A1AD83C2FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FD502A-A52A-4BF2-8812-B43D739B0DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9757,10 +9757,10 @@
   <dimension ref="A1:O734"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C102" sqref="C102"/>
+      <selection pane="bottomRight" activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14867,7 +14867,7 @@
       <c r="B107" s="38">
         <v>2</v>
       </c>
-      <c r="C107" s="22" t="s">
+      <c r="C107" s="82" t="s">
         <v>700</v>
       </c>
       <c r="D107" s="18" t="s">
@@ -16068,7 +16068,7 @@
       <c r="B132" s="38">
         <v>2</v>
       </c>
-      <c r="C132" s="18" t="s">
+      <c r="C132" s="81" t="s">
         <v>527</v>
       </c>
       <c r="D132" s="18" t="s">
@@ -16164,7 +16164,7 @@
       <c r="B134" s="38">
         <v>2</v>
       </c>
-      <c r="C134" s="18" t="s">
+      <c r="C134" s="81" t="s">
         <v>42</v>
       </c>
       <c r="D134" s="18" t="s">
@@ -16405,7 +16405,7 @@
       <c r="B139" s="38">
         <v>2</v>
       </c>
-      <c r="C139" s="18" t="s">
+      <c r="C139" s="81" t="s">
         <v>1090</v>
       </c>
       <c r="D139" s="18" t="s">
@@ -16597,7 +16597,7 @@
       <c r="B143" s="38">
         <v>2</v>
       </c>
-      <c r="C143" s="18" t="s">
+      <c r="C143" s="81" t="s">
         <v>90</v>
       </c>
       <c r="D143" s="18" t="s">

</xml_diff>

<commit_message>
several updates + script-logging
</commit_message>
<xml_diff>
--- a/1.0.4-matrix-1.3-rc/matrix/Validatiematrix_v1.3-rc.xlsx
+++ b/1.0.4-matrix-1.3-rc/matrix/Validatiematrix_v1.3-rc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4-matrix-1.3-rc\matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62383E53-EB1A-4F37-84E3-3DC79791AE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7F46A6-DB0D-4951-A246-28B1876C106E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9827,10 +9827,10 @@
   <dimension ref="A1:P734"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E348" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E386" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D374" sqref="D374"/>
+      <selection pane="bottomRight" activeCell="D425" sqref="D425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -27894,7 +27894,7 @@
       <c r="C374" s="38">
         <v>8</v>
       </c>
-      <c r="D374" s="18" t="s">
+      <c r="D374" s="80" t="s">
         <v>647</v>
       </c>
       <c r="E374" s="18" t="s">
@@ -28182,7 +28182,7 @@
       <c r="C380" s="38">
         <v>8</v>
       </c>
-      <c r="D380" s="18" t="s">
+      <c r="D380" s="80" t="s">
         <v>1749</v>
       </c>
       <c r="E380" s="18" t="s">
@@ -28230,7 +28230,7 @@
       <c r="C381" s="38">
         <v>8</v>
       </c>
-      <c r="D381" s="18" t="s">
+      <c r="D381" s="80" t="s">
         <v>1748</v>
       </c>
       <c r="E381" s="18" t="s">
@@ -28902,7 +28902,7 @@
       <c r="C395" s="38">
         <v>8</v>
       </c>
-      <c r="D395" s="18" t="s">
+      <c r="D395" s="80" t="s">
         <v>1790</v>
       </c>
       <c r="E395" s="18" t="s">

</xml_diff>

<commit_message>
STOP0018 + scripts updates
</commit_message>
<xml_diff>
--- a/1.0.4-matrix-1.3-rc/matrix/Validatiematrix_v1.3-rc.xlsx
+++ b/1.0.4-matrix-1.3-rc/matrix/Validatiematrix_v1.3-rc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4-matrix-1.3-rc\matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520DB87F-56F2-41B3-B095-810347EC4EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A407FB4-4D11-4428-A8A9-D968A78161CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9878,10 +9878,10 @@
   <dimension ref="A1:P734"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E398" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E453" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E427" sqref="E427"/>
+      <selection pane="bottomRight" activeCell="D490" sqref="D490"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -33513,7 +33513,7 @@
       <c r="C490" s="38">
         <v>2</v>
       </c>
-      <c r="D490" s="18" t="s">
+      <c r="D490" s="79" t="s">
         <v>773</v>
       </c>
       <c r="E490" s="18" t="s">
@@ -36441,7 +36441,7 @@
       <c r="C551" s="38">
         <v>2</v>
       </c>
-      <c r="D551" s="18" t="s">
+      <c r="D551" s="79" t="s">
         <v>895</v>
       </c>
       <c r="E551" s="18" t="s">
@@ -36489,7 +36489,7 @@
       <c r="C552" s="38">
         <v>2</v>
       </c>
-      <c r="D552" s="18" t="s">
+      <c r="D552" s="79" t="s">
         <v>896</v>
       </c>
       <c r="E552" s="18" t="s">

</xml_diff>